<commit_message>
comparison prod fun , hp, cf lac 18
</commit_message>
<xml_diff>
--- a/raw_data/PIB_potencial_rm.xlsx
+++ b/raw_data/PIB_potencial_rm.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\GitHub\new_normal\raw_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>AR</t>
   </si>
@@ -83,23 +78,26 @@
     <t>2010-2016</t>
   </si>
   <si>
-    <t>lac18</t>
+    <t>iso2c</t>
   </si>
   <si>
-    <t>cardm</t>
+    <t>SV</t>
   </si>
   <si>
-    <t>sa</t>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>UY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,7 +151,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,7 +167,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -211,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,27 +241,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,24 +275,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,16 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:S28"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -553,7 +518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -612,7 +577,7 @@
         <v>1.7700674771986374E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1991</v>
       </c>
@@ -671,7 +636,7 @@
         <v>2.7656755452497683E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1992</v>
       </c>
@@ -730,7 +695,7 @@
         <v>4.1348938354919262E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1993</v>
       </c>
@@ -789,7 +754,7 @@
         <v>3.88905013631737E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -848,7 +813,7 @@
         <v>3.424733703120364E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -907,7 +872,7 @@
         <v>2.8143916243663678E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1996</v>
       </c>
@@ -966,7 +931,7 @@
         <v>1.9219026393550623E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1997</v>
       </c>
@@ -1025,7 +990,7 @@
         <v>2.7010493934759357E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1998</v>
       </c>
@@ -1084,7 +1049,7 @@
         <v>3.1924004570078421E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1999</v>
       </c>
@@ -1143,7 +1108,7 @@
         <v>2.6208302118337256E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -1202,7 +1167,7 @@
         <v>2.1484028688092256E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>2001</v>
       </c>
@@ -1261,7 +1226,7 @@
         <v>2.6229513558938891E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -1320,7 +1285,7 @@
         <v>2.9004169431401244E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1379,7 +1344,7 @@
         <v>-1.4981080656793265E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -1438,7 +1403,7 @@
         <v>1.8281228114161011E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -1497,7 +1462,7 @@
         <v>3.5548542241876542E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -1556,7 +1521,7 @@
         <v>4.8990773094106377E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -1615,7 +1580,7 @@
         <v>6.6752670553419213E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -1674,7 +1639,7 @@
         <v>7.4593671385373067E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -1733,7 +1698,7 @@
         <v>5.0108765579922235E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -1792,7 +1757,7 @@
         <v>2.8960604621144491E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -1851,7 +1816,7 @@
         <v>2.7789324554951419E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -1910,7 +1875,7 @@
         <v>3.7726281622051799E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -1969,7 +1934,7 @@
         <v>4.0291059121512034E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -2028,7 +1993,7 @@
         <v>2.4452841753430272E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>2015</v>
       </c>
@@ -2093,16 +2058,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AC19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
       <c r="B1">
         <v>1990</v>
       </c>
@@ -2181,14 +2149,8 @@
       <c r="AA1">
         <v>2015</v>
       </c>
-      <c r="AB1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2270,16 +2232,10 @@
       <c r="AA2" s="1">
         <v>2.4751768590528741E-2</v>
       </c>
-      <c r="AB2" s="2">
-        <f>AVERAGE(O2:T2)</f>
-        <v>3.9665354453587036E-2</v>
-      </c>
-      <c r="AC2" s="2">
-        <f>AVERAGE(V2:AA2)</f>
-        <v>3.9648260972045178E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2361,16 +2317,10 @@
       <c r="AA3" s="1">
         <v>6.5576551902531949E-2</v>
       </c>
-      <c r="AB3" s="2">
-        <f t="shared" ref="AB3:AB19" si="0">AVERAGE(O3:T3)</f>
-        <v>3.7845005698118196E-2</v>
-      </c>
-      <c r="AC3" s="2">
-        <f t="shared" ref="AC3:AC19" si="1">AVERAGE(V3:AA3)</f>
-        <v>6.1401524121423114E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2452,16 +2402,10 @@
       <c r="AA4" s="1">
         <v>1.0947392840120215E-2</v>
       </c>
-      <c r="AB4" s="2">
-        <f t="shared" si="0"/>
-        <v>2.896049356230199E-2</v>
-      </c>
-      <c r="AC4" s="2">
-        <f t="shared" si="1"/>
-        <v>3.262916221127956E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2543,16 +2487,10 @@
       <c r="AA5" s="1">
         <v>3.4764118952373052E-2</v>
       </c>
-      <c r="AB5" s="2">
-        <f t="shared" si="0"/>
-        <v>5.5350409067674973E-2</v>
-      </c>
-      <c r="AC5" s="2">
-        <f t="shared" si="1"/>
-        <v>4.5220948921828097E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2634,16 +2572,10 @@
       <c r="AA6" s="1">
         <v>4.8405629959296148E-2</v>
       </c>
-      <c r="AB6" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6706416786745614E-2</v>
-      </c>
-      <c r="AC6" s="2">
-        <f t="shared" si="1"/>
-        <v>5.0134972766707891E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2725,16 +2657,10 @@
       <c r="AA7" s="1">
         <v>4.6445764282193214E-2</v>
       </c>
-      <c r="AB7" s="2">
-        <f t="shared" si="0"/>
-        <v>5.9789489055427962E-2</v>
-      </c>
-      <c r="AC7" s="2">
-        <f t="shared" si="1"/>
-        <v>4.8781703286850032E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2816,18 +2742,12 @@
       <c r="AA8" s="1">
         <v>5.1213953721910219E-2</v>
       </c>
-      <c r="AB8" s="2">
-        <f t="shared" si="0"/>
-        <v>5.1712424212130549E-2</v>
-      </c>
-      <c r="AC8" s="2">
-        <f t="shared" si="1"/>
-        <v>5.6574357716879152E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>2.5412313607867863E-2</v>
@@ -2907,16 +2827,10 @@
       <c r="AA9" s="1">
         <v>1.7167793025545598E-2</v>
       </c>
-      <c r="AB9" s="2">
-        <f t="shared" si="0"/>
-        <v>2.3198715022335028E-2</v>
-      </c>
-      <c r="AC9" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7189774536864558E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2998,16 +2912,10 @@
       <c r="AA10" s="1">
         <v>4.9818157647143299E-2</v>
       </c>
-      <c r="AB10" s="2">
-        <f t="shared" si="0"/>
-        <v>5.369927437367384E-2</v>
-      </c>
-      <c r="AC10" s="2">
-        <f t="shared" si="1"/>
-        <v>3.7909571712601224E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3089,16 +2997,10 @@
       <c r="AA11" s="1">
         <v>4.4576142881562086E-2</v>
       </c>
-      <c r="AB11" s="2">
-        <f t="shared" si="0"/>
-        <v>6.0435684721835935E-2</v>
-      </c>
-      <c r="AC11" s="2">
-        <f t="shared" si="1"/>
-        <v>4.3471744473040037E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3180,16 +3082,10 @@
       <c r="AA12" s="1">
         <v>3.2797131606537265E-2</v>
       </c>
-      <c r="AB12" s="2">
-        <f t="shared" si="0"/>
-        <v>3.9041815328334388E-2</v>
-      </c>
-      <c r="AC12" s="2">
-        <f t="shared" si="1"/>
-        <v>3.2273843582091753E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3271,16 +3167,10 @@
       <c r="AA13" s="1">
         <v>5.4366504826709836E-2</v>
       </c>
-      <c r="AB13" s="2">
-        <f t="shared" si="0"/>
-        <v>5.3300850691956565E-2</v>
-      </c>
-      <c r="AC13" s="2">
-        <f t="shared" si="1"/>
-        <v>4.7787441419334463E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3362,16 +3252,10 @@
       <c r="AA14" s="1">
         <v>8.4957822629497221E-2</v>
       </c>
-      <c r="AB14" s="2">
-        <f t="shared" si="0"/>
-        <v>6.2826313037401257E-2</v>
-      </c>
-      <c r="AC14" s="2">
-        <f t="shared" si="1"/>
-        <v>8.8849303834401636E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3453,16 +3337,10 @@
       <c r="AA15" s="1">
         <v>5.9644335839389259E-2</v>
       </c>
-      <c r="AB15" s="2">
-        <f t="shared" si="0"/>
-        <v>5.5461697484229779E-2</v>
-      </c>
-      <c r="AC15" s="2">
-        <f t="shared" si="1"/>
-        <v>7.4029729921410006E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3544,18 +3422,12 @@
       <c r="AA16" s="1">
         <v>5.2653613135217409E-2</v>
       </c>
-      <c r="AB16" s="2">
-        <f t="shared" si="0"/>
-        <v>3.5149671157285671E-2</v>
-      </c>
-      <c r="AC16" s="2">
-        <f t="shared" si="1"/>
-        <v>5.2802694920651171E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>5.1877337561227352E-2</v>
@@ -3635,18 +3507,12 @@
       <c r="AA17" s="1">
         <v>5.260808167888191E-2</v>
       </c>
-      <c r="AB17" s="2">
-        <f t="shared" si="0"/>
-        <v>5.2380763654434538E-2</v>
-      </c>
-      <c r="AC17" s="2">
-        <f t="shared" si="1"/>
-        <v>5.1697683957209979E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>1.6887795410242001E-2</v>
@@ -3726,16 +3592,10 @@
       <c r="AA18" s="1">
         <v>4.3727196280999026E-2</v>
       </c>
-      <c r="AB18" s="2">
-        <f t="shared" si="0"/>
-        <v>1.9906118746560255E-2</v>
-      </c>
-      <c r="AC18" s="2">
-        <f t="shared" si="1"/>
-        <v>5.3135786009643027E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3817,29 +3677,8 @@
       <c r="AA19" s="1">
         <v>6.5265477080968708E-3</v>
       </c>
-      <c r="AB19" s="2">
-        <f t="shared" si="0"/>
-        <v>3.8197634122023823E-2</v>
-      </c>
-      <c r="AC19" s="2">
-        <f t="shared" si="1"/>
-        <v>2.7624443230197814E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="AA21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="AA22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="AA23" t="s">
-        <v>22</v>
-      </c>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3847,16 +3686,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AC19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="B1">
         <v>1990</v>
       </c>
@@ -3942,7 +3781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4053,7 +3892,7 @@
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4164,7 +4003,7 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4275,7 +4114,7 @@
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4386,7 +4225,7 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4497,7 +4336,7 @@
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4608,7 +4447,7 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4719,7 +4558,7 @@
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4830,7 +4669,7 @@
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4941,7 +4780,7 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5052,7 +4891,7 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5163,7 +5002,7 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5274,7 +5113,7 @@
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5385,7 +5224,7 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5496,7 +5335,7 @@
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5607,7 +5446,7 @@
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -5718,7 +5557,7 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5829,7 +5668,7 @@
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
         <v>17</v>
       </c>

</xml_diff>